<commit_message>
# update calibration curves version March 11, 2018
</commit_message>
<xml_diff>
--- a/lib/APGCMS/APGCMS/lib/lib_urine_CalibrationCurve_TropicAcid_20180228.xlsx
+++ b/lib/APGCMS/APGCMS/lib/lib_urine_CalibrationCurve_TropicAcid_20180228.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beomsoo/gcmsProfiling/gc-autofit/lib/APGCMS/APGCMS/lib/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C416D45E-F31C-1844-AB99-369F571C26CC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0018DEC-99FA-CB45-B3F0-8AF52EFF249D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37400" yWindow="500" windowWidth="26240" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40660" yWindow="540" windowWidth="26240" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lib_urine_CalibrationCurve_Trop" sheetId="1" r:id="rId1"/>
@@ -1183,13 +1183,13 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>